<commit_message>
leer desde una linea
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>FECHA INGRESO</t>
   </si>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Pbro. Lorenzo Pérez esq Domingo Ortíz </t>
   </si>
   <si>
-    <t>END</t>
+    <t>tipoInmueble</t>
   </si>
 </sst>
 </file>
@@ -137,13 +137,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,12 +438,12 @@
     <col min="3" max="3" width="20.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="3"/>
-    <col min="7" max="7" width="37.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="15.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,14 +462,17 @@
       <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44370</v>
       </c>
@@ -478,16 +482,14 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya guarda todo, falta estados
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>FECHA INGRESO</t>
-  </si>
-  <si>
-    <t>tipo de propiedad</t>
   </si>
   <si>
     <t>departamento</t>
@@ -76,12 +73,36 @@
   <si>
     <t>tipoInmueble</t>
   </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1oV-qfNcAfP5WEQCiXlzBzbdhoTHAreQw?usp=sharing</t>
+  </si>
+  <si>
+    <t>FOTOS</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1v7MA25xW1gwBp8rHIVLuGRCnFTnmH5aV?usp=sharing</t>
+  </si>
+  <si>
+    <t>Gs. 1.000.000</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>USD 20.000</t>
+  </si>
+  <si>
+    <t>15 de Agosto N° 230 entre Palma y Pte. Franco</t>
+  </si>
+  <si>
+    <t>test Monoambiente con un baño y balcón a la calle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +125,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +159,12 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -137,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -145,6 +186,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,75 +470,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="15.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="37.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>12</v>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44370</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>38119</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ya guarda todo con estados
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>FECHA INGRESO</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>test Monoambiente con un baño y balcón a la calle</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>disponible</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +495,7 @@
     <col min="9" max="9" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,8 +523,11 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44370</v>
       </c>
@@ -537,8 +546,11 @@
       <c r="I2" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>38119</v>
       </c>
@@ -566,6 +578,7 @@
       <c r="I3" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="J3" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>